<commit_message>
Player 회피 추가, PlayerDodgeDurationTime 시트 데이터 추가, PlayerDodgeAddForce 시트데이터 추가, Player Bat Angle 기준 축 변경, (Player,Enemy,Ball)예전 코드 삭제
</commit_message>
<xml_diff>
--- a/_GameData/CharacterGameData.xlsx
+++ b/_GameData/CharacterGameData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\224dj\Desktop\테이블\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matiy\OneDrive\Desktop\Unity\QT_Proto\_GameData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{46179758-A41D-4BC0-823A-719306D62BA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87584A6F-3835-4AEC-AE28-2407E9C3B59A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6E11533B-0F9C-4925-AEFA-43AC370FE899}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{6E11533B-0F9C-4925-AEFA-43AC370FE899}"/>
   </bookViews>
   <sheets>
     <sheet name="CharacterGameData" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t>int</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -103,6 +103,14 @@
   </si>
   <si>
     <t>주인공</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DodgeAddForce</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DodgeDurationTime</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -286,9 +294,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{14AA5828-211A-4638-8049-D1EE1954BC2E}" name="CharacterTable" displayName="CharacterTable" ref="B2:N3" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="B2:N3" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
-  <tableColumns count="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{14AA5828-211A-4638-8049-D1EE1954BC2E}" name="CharacterTable" displayName="CharacterTable" ref="B2:P3" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="B2:P3" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+  <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{D54F1EF8-5CA3-42E3-9298-39DB0F04B351}" name="Index"/>
     <tableColumn id="12" xr3:uid="{55133BB9-5092-4B72-81EB-5DF0229ABFF1}" name="#설명" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{652E5535-93BF-4721-B457-6E4283E0A341}" name="MaxHP"/>
@@ -298,6 +306,8 @@
     <tableColumn id="5" xr3:uid="{824F9C0B-5423-4353-B9A2-5044E8CF7FDF}" name="MercyInvincibleTime"/>
     <tableColumn id="6" xr3:uid="{06FF55BB-F4EB-4DAF-B063-9F292E82E636}" name="DodgeCooldown"/>
     <tableColumn id="7" xr3:uid="{5CAA1ECF-BA76-4413-8EE5-41D548F52919}" name="DodgeInvincibleTime"/>
+    <tableColumn id="16" xr3:uid="{CF4860D1-8036-42CB-A534-B8F526AE37B7}" name="DodgeDurationTime"/>
+    <tableColumn id="15" xr3:uid="{414C6B80-2F05-44FA-8583-0DF5A39D0B14}" name="DodgeAddForce"/>
     <tableColumn id="8" xr3:uid="{12F774CF-EB11-4446-90E3-1F696E8AED07}" name="ItemSlotMax"/>
     <tableColumn id="9" xr3:uid="{8720F719-56E9-4229-840A-1EA2AEFB6D70}" name="BallStackMax"/>
     <tableColumn id="10" xr3:uid="{AC240661-1619-4AA9-ACC6-2A7B7DBCA72D}" name="GoldGain"/>
@@ -607,10 +617,10 @@
   <sheetPr codeName="Sheet3">
     <tabColor theme="5" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="B1:N3"/>
+  <dimension ref="B1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -624,13 +634,15 @@
     <col min="8" max="8" width="22.875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.75" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="23.375" customWidth="1"/>
+    <col min="13" max="13" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14">
+    <row r="1" spans="2:16">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -659,10 +671,10 @@
         <v>2</v>
       </c>
       <c r="K1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M1" t="s">
         <v>0</v>
@@ -670,8 +682,14 @@
       <c r="N1" t="s">
         <v>0</v>
       </c>
+      <c r="O1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P1" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="2" spans="2:14">
+    <row r="2" spans="2:16">
       <c r="B2" t="s">
         <v>3</v>
       </c>
@@ -700,19 +718,25 @@
         <v>11</v>
       </c>
       <c r="K2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" t="s">
         <v>12</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>13</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>14</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="2:14">
+    <row r="3" spans="2:16">
       <c r="B3">
         <v>100</v>
       </c>
@@ -726,7 +750,7 @@
         <v>5</v>
       </c>
       <c r="F3">
-        <v>300</v>
+        <v>7</v>
       </c>
       <c r="G3">
         <v>200</v>
@@ -741,15 +765,21 @@
         <v>0.3</v>
       </c>
       <c r="K3">
+        <v>0.3</v>
+      </c>
+      <c r="L3">
+        <v>12</v>
+      </c>
+      <c r="M3">
         <v>10</v>
       </c>
-      <c r="L3">
+      <c r="N3">
         <v>1</v>
       </c>
-      <c r="M3">
+      <c r="O3">
         <v>1</v>
       </c>
-      <c r="N3">
+      <c r="P3">
         <v>200</v>
       </c>
     </row>

</xml_diff>